<commit_message>
Initial full project upload after repo reset
</commit_message>
<xml_diff>
--- a/temp_qc_domain_output.xlsx
+++ b/temp_qc_domain_output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="147">
   <si>
     <t>Id</t>
   </si>
@@ -253,18 +253,6 @@
     <t>Data Source</t>
   </si>
   <si>
-    <t>discovered_employees</t>
-  </si>
-  <si>
-    <t>discovered_revenue</t>
-  </si>
-  <si>
-    <t>discovered_industry</t>
-  </si>
-  <si>
-    <t>flagged_rpe</t>
-  </si>
-  <si>
     <t>email_status_Classification</t>
   </si>
   <si>
@@ -274,6 +262,12 @@
     <t>Reason_for_domain_mismatch_mail</t>
   </si>
   <si>
+    <t>WorkPhone_Reason</t>
+  </si>
+  <si>
+    <t>WorkPhone_ColorFlag</t>
+  </si>
+  <si>
     <t>linkedin_link_found</t>
   </si>
   <si>
@@ -445,16 +439,10 @@
     <t>133</t>
   </si>
   <si>
-    <t>44 employees</t>
-  </si>
-  <si>
-    <t>Truck Transportation</t>
+    <t>Match</t>
   </si>
   <si>
     <t>False</t>
-  </si>
-  <si>
-    <t>Match</t>
   </si>
   <si>
     <t>Hansen &amp; Adkins - Transportation service in Los Alamitos, California</t>
@@ -837,13 +825,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CP2"/>
+  <dimension ref="A1:CN2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:94">
+    <row r="1" spans="1:92">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1120,212 +1108,200 @@
       <c r="CN1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="CO1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:92">
+      <c r="A2" t="s">
         <v>92</v>
       </c>
-      <c r="CP1" s="1" t="s">
+      <c r="B2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="2" spans="1:94">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
         <v>94</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>95</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>96</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>97</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H2" t="s">
         <v>98</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>99</v>
       </c>
-      <c r="G2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>100</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>101</v>
       </c>
-      <c r="J2" t="s">
+      <c r="N2" t="s">
         <v>102</v>
       </c>
-      <c r="K2" t="s">
+      <c r="O2" t="s">
         <v>103</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>104</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>105</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>106</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>107</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>108</v>
       </c>
-      <c r="S2" t="s">
+      <c r="U2" t="s">
         <v>109</v>
       </c>
-      <c r="T2" t="s">
+      <c r="V2" t="s">
         <v>110</v>
       </c>
-      <c r="U2" t="s">
+      <c r="W2" t="s">
         <v>111</v>
       </c>
-      <c r="V2" t="s">
+      <c r="Y2" t="s">
         <v>112</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Z2" t="s">
         <v>113</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AA2" t="s">
         <v>114</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AB2" t="s">
         <v>115</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AC2" t="s">
         <v>116</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AE2" t="s">
         <v>117</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AH2" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AJ2" t="s">
         <v>119</v>
       </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AK2" t="s">
         <v>120</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AN2" t="s">
         <v>121</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AO2" t="s">
         <v>122</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AP2" t="s">
         <v>123</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AQ2" t="s">
+        <v>122</v>
+      </c>
+      <c r="AU2" t="s">
         <v>124</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AV2" t="s">
         <v>125</v>
       </c>
-      <c r="AQ2" t="s">
-        <v>124</v>
-      </c>
-      <c r="AU2" t="s">
+      <c r="AW2" t="s">
         <v>126</v>
       </c>
-      <c r="AV2" t="s">
+      <c r="AX2" t="s">
         <v>127</v>
       </c>
-      <c r="AW2" t="s">
+      <c r="AY2" t="s">
         <v>128</v>
       </c>
-      <c r="AX2" t="s">
+      <c r="BB2" t="s">
+        <v>119</v>
+      </c>
+      <c r="BC2" t="s">
         <v>129</v>
       </c>
-      <c r="AY2" t="s">
+      <c r="BD2" t="s">
         <v>130</v>
       </c>
-      <c r="BB2" t="s">
-        <v>121</v>
-      </c>
-      <c r="BC2" t="s">
+      <c r="BE2" t="s">
         <v>131</v>
       </c>
-      <c r="BD2" t="s">
+      <c r="BF2" t="s">
         <v>132</v>
       </c>
-      <c r="BE2" t="s">
+      <c r="BI2" t="s">
         <v>133</v>
       </c>
-      <c r="BF2" t="s">
+      <c r="BN2" t="s">
         <v>134</v>
       </c>
-      <c r="BI2" t="s">
+      <c r="BO2" t="s">
         <v>135</v>
       </c>
-      <c r="BN2" t="s">
+      <c r="BP2" t="s">
         <v>136</v>
       </c>
-      <c r="BO2" t="s">
+      <c r="BQ2" t="s">
         <v>137</v>
       </c>
-      <c r="BP2" t="s">
+      <c r="BT2" t="s">
         <v>138</v>
       </c>
-      <c r="BQ2" t="s">
+      <c r="BY2" t="s">
         <v>139</v>
       </c>
-      <c r="BT2" t="s">
+      <c r="BZ2" t="s">
         <v>140</v>
       </c>
-      <c r="BY2" t="s">
+      <c r="CB2" t="s">
         <v>141</v>
       </c>
-      <c r="BZ2" t="s">
+      <c r="CF2" t="s">
         <v>142</v>
       </c>
-      <c r="CB2" t="s">
+      <c r="CG2" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="CH2" t="s">
+        <v>94</v>
+      </c>
+      <c r="CI2" t="s">
+        <v>116</v>
+      </c>
+      <c r="CJ2" t="s">
+        <v>116</v>
+      </c>
+      <c r="CK2" t="s">
         <v>143</v>
       </c>
-      <c r="CD2" t="s">
+      <c r="CL2" t="s">
         <v>144</v>
       </c>
-      <c r="CE2" t="s">
+      <c r="CM2" t="s">
         <v>145</v>
       </c>
-      <c r="CF2" t="s">
+      <c r="CN2" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="CI2" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="CJ2" t="s">
-        <v>96</v>
-      </c>
-      <c r="CK2" t="s">
-        <v>118</v>
-      </c>
-      <c r="CL2" t="s">
-        <v>118</v>
-      </c>
-      <c r="CM2" t="s">
-        <v>147</v>
-      </c>
-      <c r="CN2" t="s">
-        <v>148</v>
-      </c>
-      <c r="CO2" t="s">
-        <v>149</v>
-      </c>
-      <c r="CP2" s="2" t="s">
-        <v>150</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="AH2" r:id="rId1"/>
-    <hyperlink ref="CI2" r:id="rId2"/>
-    <hyperlink ref="CP2" r:id="rId3"/>
+    <hyperlink ref="CG2" r:id="rId2"/>
+    <hyperlink ref="CN2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>